<commit_message>
Deployed e97fb56 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA qPCR/example output/Results_edited.xlsx
+++ b/eDNA qPCR/example output/Results_edited.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\github\resources\docs\eDNA qPCR\example output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD9874E-13FD-4E63-8640-0C18629C862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B44A639-0A00-47C5-9205-C3789A860E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="12768" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1492,16 +1492,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11:T14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P150" sqref="P150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.77734375" customWidth="1"/>
-    <col min="15" max="15" width="24.44140625" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="54.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>